<commit_message>
updated with RQ1 results
</commit_message>
<xml_diff>
--- a/data/scopus_outputs_2/paper_stats.xlsx
+++ b/data/scopus_outputs_2/paper_stats.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11027"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erinbuchanan/GitHub/Research/2_projects/big_team_who/data/scopus_outputs_2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3129C2B7-80B7-B34F-9A50-FA2B8CFB24B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41BD3CD8-4CCF-8147-925C-221CC20B5A6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25600" yWindow="-1460" windowWidth="25600" windowHeight="13900" xr2:uid="{0151A648-758E-034D-85F4-AA7C0A48B8EE}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{0151A648-758E-034D-85F4-AA7C0A48B8EE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -65,13 +65,13 @@
     <t>Authors</t>
   </si>
   <si>
-    <t>6+</t>
-  </si>
-  <si>
     <t>50+</t>
   </si>
   <si>
     <t>100+</t>
+  </si>
+  <si>
+    <t>11+</t>
   </si>
 </sst>
 </file>
@@ -453,7 +453,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="18.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -505,7 +505,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
@@ -525,7 +525,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B5" t="s">
         <v>8</v>
@@ -545,7 +545,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B6" t="s">
         <v>7</v>
@@ -565,7 +565,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7" t="s">
         <v>8</v>
@@ -585,7 +585,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B8" t="s">
         <v>7</v>
@@ -605,7 +605,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B9" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
add new files for finalized data
</commit_message>
<xml_diff>
--- a/data/scopus_outputs_2/paper_stats.xlsx
+++ b/data/scopus_outputs_2/paper_stats.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10511"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erinbuchanan/GitHub/Research/2_projects/big_team_who/data/scopus_outputs_2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41BD3CD8-4CCF-8147-925C-221CC20B5A6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C07579D8-E4F4-9C48-AF35-73B72A6CD3D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{0151A648-758E-034D-85F4-AA7C0A48B8EE}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="15120" windowHeight="18880" xr2:uid="{0151A648-758E-034D-85F4-AA7C0A48B8EE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -452,8 +452,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E32732E-ECB4-AC4D-BA39-EB72939D2430}">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="18.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -493,7 +493,18 @@
       <c r="B2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="1"/>
+      <c r="C2" s="1">
+        <v>8758846</v>
+      </c>
+      <c r="D2">
+        <v>17195880</v>
+      </c>
+      <c r="E2">
+        <v>3441064</v>
+      </c>
+      <c r="F2">
+        <v>8705266</v>
+      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -501,6 +512,18 @@
       </c>
       <c r="B3" t="s">
         <v>8</v>
+      </c>
+      <c r="C3">
+        <v>12096908</v>
+      </c>
+      <c r="D3">
+        <v>15366570</v>
+      </c>
+      <c r="E3">
+        <v>5182626</v>
+      </c>
+      <c r="F3">
+        <v>11557780</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">

</xml_diff>